<commit_message>
transcription update - incomplete
</commit_message>
<xml_diff>
--- a/data/trasncription_ex2.xlsx
+++ b/data/trasncription_ex2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/serenekim/Library/CloudStorage/OneDrive-VrijeUniversiteitBrussel/img-analysis_seorin_project/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vub-my.sharepoint.com/personal/seorin_kim_vub_be/Documents/img-analysis_seorin_project/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{599DD264-B8F2-8146-B6C1-713C651506D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{599DD264-B8F2-8146-B6C1-713C651506D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1209DE50-4984-DC49-B081-CC828358C105}"/>
   <bookViews>
-    <workbookView xWindow="14120" yWindow="2040" windowWidth="30240" windowHeight="18880" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
+    <workbookView xWindow="0" yWindow="760" windowWidth="30240" windowHeight="18880" xr2:uid="{6D6EFBF4-D3F9-A04D-9AC4-202B897D114E}"/>
   </bookViews>
   <sheets>
     <sheet name="IMG_2024_03_19_11_45_57_427" sheetId="2" r:id="rId1"/>
@@ -65,7 +65,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
   <si>
     <t>Nom.</t>
   </si>
@@ -289,99 +289,118 @@
     <t>Oisquercq</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>Tubize</t>
   </si>
   <si>
     <t>Allard Marie</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Ronsmans </t>
-    </r>
+    <t>? / 1921</t>
+  </si>
+  <si>
+    <t>191/1919</t>
+  </si>
+  <si>
+    <t>16 9b 1919</t>
+  </si>
+  <si>
+    <t>14 mars 1928</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>16 "</t>
+  </si>
+  <si>
+    <t>4 janvier 1928</t>
+  </si>
+  <si>
+    <t>17 9b 1919</t>
+  </si>
+  <si>
+    <t>24 avril 1919</t>
+  </si>
+  <si>
+    <t>17 9bre 1919</t>
+  </si>
+  <si>
+    <t>7 avril 1920</t>
+  </si>
+  <si>
+    <t>19 9bre 1919</t>
+  </si>
+  <si>
+    <t>15 avril 1919</t>
+  </si>
+  <si>
+    <t>19 "</t>
+  </si>
+  <si>
+    <t>14 juin 1920</t>
+  </si>
+  <si>
+    <t>20 "</t>
+  </si>
+  <si>
+    <t>16 mars 1920</t>
+  </si>
+  <si>
+    <t>10 9b 1920</t>
+  </si>
+  <si>
+    <t>non passible</t>
+  </si>
+  <si>
+    <t>16 fevrier 1920</t>
+  </si>
+  <si>
+    <t>13 mars 1923</t>
+  </si>
+  <si>
+    <t>29 9b 1923</t>
+  </si>
+  <si>
+    <t>Monstreux</t>
+  </si>
+  <si>
+    <t>16 avril 1919</t>
+  </si>
+  <si>
+    <t>19 octobre 1918</t>
+  </si>
+  <si>
+    <t>Waterloo</t>
+  </si>
+  <si>
+    <t>Ronsmans Armande</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <sz val="12"/>
         <color rgb="FFFF0000"/>
         <rFont val="Aptos Narrow (Body)"/>
       </rPr>
-      <t>?</t>
+      <t>Vusseke</t>
     </r>
-  </si>
-  <si>
-    <t>? / 1921</t>
-  </si>
-  <si>
-    <t>191/1919</t>
-  </si>
-  <si>
-    <t>16 9b 1919</t>
-  </si>
-  <si>
-    <t>14 mars 1928</t>
-  </si>
-  <si>
-    <t>"</t>
-  </si>
-  <si>
-    <t>16 "</t>
-  </si>
-  <si>
-    <t>4 janvier 1928</t>
-  </si>
-  <si>
-    <t>17 9b 1919</t>
-  </si>
-  <si>
-    <t>24 avril 1919</t>
-  </si>
-  <si>
-    <t>17 9bre 1919</t>
-  </si>
-  <si>
-    <t>7 avril 1920</t>
-  </si>
-  <si>
-    <t>19 9bre 1919</t>
-  </si>
-  <si>
-    <t>15 avril 1919</t>
-  </si>
-  <si>
-    <t>19 "</t>
-  </si>
-  <si>
-    <t>14 juin 1920</t>
-  </si>
-  <si>
-    <t>20 "</t>
-  </si>
-  <si>
-    <t>16 mars 1920</t>
-  </si>
-  <si>
-    <t>10 9b 1920</t>
-  </si>
-  <si>
-    <t>non passible</t>
-  </si>
-  <si>
-    <t>16 fevrier 1920</t>
-  </si>
-  <si>
-    <t>13 mars 1923</t>
-  </si>
-  <si>
-    <t>29 9b 1923</t>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> Edouard</t>
+    </r>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -408,12 +427,6 @@
       <color rgb="FFFF0000"/>
       <name val="Aptos Narrow (Body)"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Tahoma"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -573,7 +586,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
@@ -605,7 +618,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -963,8 +975,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DB076F5B-4564-1543-8968-7E29FE54F40E}">
   <dimension ref="A1:U19"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="131" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" zoomScale="131" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1122,14 +1134,14 @@
       </c>
       <c r="L4" s="2"/>
       <c r="M4" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="N4" s="1"/>
       <c r="O4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="Q4" s="2"/>
       <c r="T4" s="2"/>
@@ -1186,18 +1198,18 @@
       </c>
       <c r="L6" s="2"/>
       <c r="M6" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="N6" s="1"/>
       <c r="O6" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P6" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q6" s="2"/>
-      <c r="R6" s="19" t="s">
-        <v>95</v>
+      <c r="R6" t="s">
+        <v>93</v>
       </c>
       <c r="S6" s="1">
         <v>872</v>
@@ -1222,7 +1234,9 @@
       <c r="G7" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="H7" s="2"/>
+      <c r="H7" s="2" t="s">
+        <v>103</v>
+      </c>
       <c r="I7">
         <v>500</v>
       </c>
@@ -1232,14 +1246,14 @@
       <c r="L7" s="2"/>
       <c r="N7" s="1"/>
       <c r="O7" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="P7" s="1" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="Q7" s="2"/>
       <c r="R7" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S7" s="1"/>
       <c r="T7" s="2"/>
@@ -1297,14 +1311,14 @@
       <c r="L9" s="2"/>
       <c r="N9" s="1"/>
       <c r="O9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="P9" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="Q9" s="2"/>
       <c r="R9" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S9" s="1"/>
       <c r="T9" s="2"/>
@@ -1324,7 +1338,7 @@
         <v>52</v>
       </c>
       <c r="E10" t="s">
-        <v>73</v>
+        <v>98</v>
       </c>
       <c r="F10" s="1"/>
       <c r="G10" s="2" t="s">
@@ -1337,14 +1351,14 @@
       <c r="L10" s="2"/>
       <c r="N10" s="1"/>
       <c r="O10" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="P10" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="Q10" s="2"/>
       <c r="R10" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="S10" s="1">
         <v>37</v>
@@ -1366,7 +1380,7 @@
         <v>57</v>
       </c>
       <c r="E11" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F11" s="1"/>
       <c r="G11" s="2" t="s">
@@ -1384,14 +1398,14 @@
       <c r="L11" s="2"/>
       <c r="N11" s="1"/>
       <c r="O11" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="P11" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="Q11" s="2"/>
       <c r="R11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S11" s="1"/>
       <c r="T11" s="2"/>
@@ -1470,12 +1484,14 @@
         <v>64</v>
       </c>
       <c r="E15" s="13" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="F15" s="1"/>
-      <c r="G15" s="2"/>
+      <c r="G15" s="2" t="s">
+        <v>100</v>
+      </c>
       <c r="H15" s="2" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="I15" s="13">
         <v>378</v>
@@ -1489,14 +1505,14 @@
       <c r="L15" s="2"/>
       <c r="N15" s="1"/>
       <c r="O15" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="P15" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="Q15" s="2"/>
       <c r="R15" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="S15" s="1"/>
       <c r="T15" s="2"/>
@@ -1516,9 +1532,11 @@
         <v>29</v>
       </c>
       <c r="F16" s="1"/>
-      <c r="G16" s="2"/>
+      <c r="G16" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="H16" s="2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I16">
         <v>7310</v>
@@ -1529,14 +1547,14 @@
       <c r="L16" s="2"/>
       <c r="N16" s="1"/>
       <c r="O16" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="P16" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="Q16" s="2"/>
       <c r="R16" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="S16" s="1">
         <v>54</v>
@@ -1576,6 +1594,9 @@
       <c r="D18" t="s">
         <v>69</v>
       </c>
+      <c r="E18" t="s">
+        <v>101</v>
+      </c>
       <c r="F18" s="1"/>
       <c r="G18" s="2" t="s">
         <v>70</v>
@@ -1595,14 +1616,14 @@
       <c r="L18" s="2"/>
       <c r="N18" s="1"/>
       <c r="O18" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="P18" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="Q18" s="2"/>
       <c r="R18" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="S18" s="1">
         <v>292</v>

</xml_diff>